<commit_message>
"Solutions of homeworks, sylabus edited"
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\elvin_taghizade\IdeaProjects\mine\git\java-course-1-classes\src\main\java\org\eminera\_syllabus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\courses\java_group_1\classes\src\main\java\org\eminera\_syllabus\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788715E4-2365-4DC6-86F7-F905968FA41D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>A. Basic / Syntax</t>
   </si>
@@ -99,13 +100,19 @@
   </si>
   <si>
     <t>final exam</t>
+  </si>
+  <si>
+    <t>String basicsc</t>
+  </si>
+  <si>
+    <t>09/31/2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -559,14 +566,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.7109375" style="20" bestFit="1" customWidth="1"/>
@@ -577,7 +584,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.5">
+    <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -597,7 +604,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -617,7 +624,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
       <c r="B3" s="7">
         <f>B2+1</f>
@@ -636,7 +643,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>
       <c r="B4" s="7">
         <f t="shared" ref="B4:B5" si="0">B3+1</f>
@@ -655,7 +662,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="38.25">
+    <row r="5" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
       <c r="B5" s="7">
         <f t="shared" si="0"/>
@@ -674,7 +681,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="26.25">
+    <row r="6" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="7">
         <f>B5+1</f>
@@ -693,7 +700,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15">
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="7">
         <f>B6+1</f>
@@ -712,7 +719,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15">
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="17"/>
       <c r="B8" s="19">
         <v>7</v>
@@ -730,7 +737,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="17"/>
       <c r="B9" s="19">
         <v>8</v>
@@ -746,13 +753,13 @@
       </c>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="17"/>
       <c r="B10" s="19">
         <v>9</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D10" s="19">
         <v>2</v>
@@ -762,33 +769,49 @@
       </c>
       <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="17"/>
-      <c r="B11" s="23">
+      <c r="B11" s="19">
         <v>10</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="19">
+        <v>2</v>
+      </c>
+      <c r="E11" s="14">
+        <v>44102</v>
+      </c>
+      <c r="F11" s="17"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="17"/>
+      <c r="B12" s="23">
+        <v>11</v>
+      </c>
+      <c r="C12" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="23">
-        <v>2</v>
-      </c>
-      <c r="E11" s="24">
-        <v>44102</v>
-      </c>
-      <c r="F11" s="21" t="s">
+      <c r="D12" s="23">
+        <v>2</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="21" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1"/>
-    <hyperlink ref="F4" r:id="rId2"/>
-    <hyperlink ref="F2" r:id="rId3"/>
-    <hyperlink ref="F5" r:id="rId4"/>
-    <hyperlink ref="F6" r:id="rId5"/>
-    <hyperlink ref="F7" r:id="rId6"/>
-    <hyperlink ref="F8" r:id="rId7"/>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>

</xml_diff>

<commit_message>
course_details.xlsx polished a bit
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -123,7 +123,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="D\-MMM\-YY"/>
+    <numFmt numFmtId="165" formatCode="d\-mmm\-yy"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -222,7 +222,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -237,6 +237,13 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -367,7 +374,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -389,13 +396,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -467,19 +474,19 @@
   </sheetPr>
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="3.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="35.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="9.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="15.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="60.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -671,7 +678,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="18"/>
       <c r="B11" s="19" t="n">
         <v>10</v>
@@ -689,7 +696,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="18"/>
       <c r="B12" s="19" t="n">
         <v>11</v>
@@ -707,7 +714,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="18"/>
       <c r="B13" s="19" t="n">
         <v>12</v>

</xml_diff>

<commit_message>
structure changed a bit
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -115,6 +115,21 @@
   </si>
   <si>
     <t xml:space="preserve">final exam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B. OOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OOP #1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OOP #2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OOP #3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OOP #4</t>
   </si>
 </sst>
 </file>
@@ -273,7 +288,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -392,6 +407,22 @@
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -472,10 +503,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -755,6 +786,64 @@
       <c r="D15" s="26"/>
       <c r="E15" s="28"/>
       <c r="F15" s="29"/>
+    </row>
+    <row r="17" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="31" t="n">
+        <v>14</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="31" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" s="33"/>
+      <c r="F17" s="30"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="30"/>
+      <c r="B18" s="31" t="n">
+        <v>14</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="31" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" s="33"/>
+      <c r="F18" s="30"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="30"/>
+      <c r="B19" s="31" t="n">
+        <v>14</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="31" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" s="33"/>
+      <c r="F19" s="30"/>
+    </row>
+    <row r="20" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="30"/>
+      <c r="B20" s="31" t="n">
+        <v>14</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="31" t="n">
+        <v>2</v>
+      </c>
+      <c r="E20" s="33"/>
+      <c r="F20" s="30"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Syllabus refreshed a bit
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -111,16 +111,82 @@
     <t xml:space="preserve">Practice – recap </t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">part #1: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://youtu.be/lumo7DTIkqg
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Part #2: https://youtu.be/oa5ZQM38AxE
+part #3: https://youtu.be/37u5R1Yy9sk</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Recap + final exam</t>
   </si>
   <si>
-    <t xml:space="preserve">final exam</t>
+    <t xml:space="preserve">https://youtu.be/ktMAcL9ksqE</t>
   </si>
   <si>
     <t xml:space="preserve">B. OOP</t>
   </si>
   <si>
     <t xml:space="preserve">OOP #1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">part #1: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://youtu.be/yvlL4xzinS8
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Part #2: https://youtu.be/xiiIKctxxcw
+part #3: https://youtu.be/7ANEfutCOVU</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">OOP #2</t>
@@ -138,9 +204,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="d\-mmm\-yy"/>
+    <numFmt numFmtId="165" formatCode="D\-MMM\-YY"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -199,6 +265,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -288,7 +360,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -393,19 +465,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -427,13 +515,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -503,13 +591,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="3.7"/>
@@ -517,7 +605,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="9.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="15.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="60.3"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -745,106 +833,118 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18"/>
+    <row r="13" s="29" customFormat="true" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="26"/>
       <c r="B13" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="27" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="19" t="n">
         <v>2</v>
       </c>
       <c r="E13" s="15" t="n">
-        <v>44472</v>
-      </c>
-      <c r="F13" s="25"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>44503</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="18"/>
-      <c r="B14" s="26" t="n">
+      <c r="B14" s="30" t="n">
         <v>13</v>
       </c>
-      <c r="C14" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="E14" s="28" t="n">
+      <c r="C14" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" s="32" t="n">
         <v>44142</v>
       </c>
-      <c r="F14" s="29" t="s">
-        <v>30</v>
+      <c r="F14" s="25" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="18"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="31" t="n">
+      <c r="B15" s="30"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="33"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="32"/>
+    </row>
+    <row r="17" customFormat="false" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="35" t="n">
         <v>14</v>
       </c>
-      <c r="C17" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="31" t="n">
-        <v>2</v>
-      </c>
-      <c r="E17" s="33"/>
-      <c r="F17" s="30"/>
+      <c r="C17" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" s="15" t="n">
+        <v>44144</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="30"/>
-      <c r="B18" s="31" t="n">
+      <c r="A18" s="34"/>
+      <c r="B18" s="35" t="n">
         <v>14</v>
       </c>
-      <c r="C18" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="31" t="n">
-        <v>2</v>
-      </c>
-      <c r="E18" s="33"/>
-      <c r="F18" s="30"/>
+      <c r="C18" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" s="37"/>
+      <c r="F18" s="34"/>
     </row>
     <row r="19" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="30"/>
-      <c r="B19" s="31" t="n">
+      <c r="A19" s="34"/>
+      <c r="B19" s="35" t="n">
         <v>14</v>
       </c>
-      <c r="C19" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="31" t="n">
-        <v>2</v>
-      </c>
-      <c r="E19" s="33"/>
-      <c r="F19" s="30"/>
+      <c r="C19" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" s="37"/>
+      <c r="F19" s="34"/>
     </row>
     <row r="20" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="30"/>
-      <c r="B20" s="31" t="n">
+      <c r="A20" s="34"/>
+      <c r="B20" s="35" t="n">
         <v>14</v>
       </c>
-      <c r="C20" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="31" t="n">
-        <v>2</v>
-      </c>
-      <c r="E20" s="33"/>
-      <c r="F20" s="30"/>
-    </row>
+      <c r="C20" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="E20" s="37"/>
+      <c r="F20" s="34"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="https://youtu.be/3Q7s1cpByuk"/>

</xml_diff>

<commit_message>
excel file updated and slides attached!
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">Arrays - Problem Solving</t>
   </si>
   <si>
-    <t xml:space="preserve">video crashed</t>
+    <t xml:space="preserve">video crashed :(</t>
   </si>
   <si>
     <t xml:space="preserve">Arrays - part 2</t>
@@ -111,37 +111,9 @@
     <t xml:space="preserve">Practice – recap </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">part #1: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://youtu.be/lumo7DTIkqg
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Part #2: https://youtu.be/oa5ZQM38AxE
+    <t xml:space="preserve">part #1: https://youtu.be/lumo7DTIkqg
+Part #2: https://youtu.be/oa5ZQM38AxE
 part #3: https://youtu.be/37u5R1Yy9sk</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Recap + final exam</t>
@@ -156,40 +128,15 @@
     <t xml:space="preserve">OOP #1</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">part #1: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://youtu.be/yvlL4xzinS8
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Part #2: https://youtu.be/xiiIKctxxcw
+    <t xml:space="preserve">part #1: https://youtu.be/yvlL4xzinS8
+Part #2: https://youtu.be/xiiIKctxxcw
 part #3: https://youtu.be/7ANEfutCOVU</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">OOP #2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part #1: Part #2:</t>
   </si>
   <si>
     <t xml:space="preserve">OOP #3</t>
@@ -204,9 +151,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="D\-MMM\-YY"/>
+    <numFmt numFmtId="165" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -265,12 +212,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -360,7 +301,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -481,19 +422,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -509,19 +450,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -593,11 +538,11 @@
   </sheetPr>
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="3.7"/>
@@ -605,7 +550,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="9.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="15.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="60.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -761,7 +706,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" s="24" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="24" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="21"/>
       <c r="B9" s="22" t="n">
         <v>8</v>
@@ -878,9 +823,14 @@
       <c r="F15" s="33"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E16" s="32"/>
-    </row>
-    <row r="17" customFormat="false" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="34"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="34"/>
+    </row>
+    <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="34" t="s">
         <v>32</v>
       </c>
@@ -900,10 +850,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="34"/>
       <c r="B18" s="35" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C18" s="36" t="s">
         <v>35</v>
@@ -911,35 +861,41 @@
       <c r="D18" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="E18" s="37"/>
-      <c r="F18" s="34"/>
-    </row>
-    <row r="19" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="15" t="n">
+        <v>44151</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="34"/>
       <c r="B19" s="35" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D19" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="E19" s="37"/>
+      <c r="E19" s="15" t="n">
+        <v>44156</v>
+      </c>
       <c r="F19" s="34"/>
     </row>
     <row r="20" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="34"/>
       <c r="B20" s="35" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D20" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="E20" s="37"/>
+      <c r="E20" s="38"/>
       <c r="F20" s="34"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Lesson %15 video material upload to youtube, more info in excel file
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -136,7 +136,8 @@
     <t xml:space="preserve">OOP #2</t>
   </si>
   <si>
-    <t xml:space="preserve">Part #1: Part #2:</t>
+    <t xml:space="preserve">Part #1: https://youtu.be/LfqWPBOWBtk
+Part #2: https://youtu.be/sqrsc7McCWc</t>
   </si>
   <si>
     <t xml:space="preserve">OOP #3</t>
@@ -151,7 +152,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="d\-mmm\-yy"/>
+    <numFmt numFmtId="165" formatCode="D\-MMM\-YY"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -460,13 +461,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -539,10 +540,10 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="3.7"/>
@@ -550,7 +551,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="9.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="15.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="60.3"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,7 +851,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="34"/>
       <c r="B18" s="35" t="n">
         <v>15</v>
@@ -864,7 +865,7 @@
       <c r="E18" s="15" t="n">
         <v>44151</v>
       </c>
-      <c r="F18" s="34" t="s">
+      <c r="F18" s="36" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Lesson #16 video material upload to youtube, more info in excel file
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t xml:space="preserve">OOP #3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part #1: https://youtu.be/Adstn_hqvJg
+Part #2: https://youtu.be/HbMFNIIB-V4
+Part #3: https://youtu.be/CzmM2m1ouaI
+Part #4: https://youtu.be/ZWD2dJoyuGQ</t>
   </si>
   <si>
     <t xml:space="preserve">OOP #4</t>
@@ -302,7 +308,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -452,10 +458,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -540,7 +542,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
+      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -869,7 +871,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="34"/>
       <c r="B19" s="35" t="n">
         <v>16</v>
@@ -883,20 +885,24 @@
       <c r="E19" s="15" t="n">
         <v>44156</v>
       </c>
-      <c r="F19" s="34"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F19" s="36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="34"/>
       <c r="B20" s="35" t="n">
         <v>17</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D20" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="E20" s="38"/>
+      <c r="E20" s="15" t="n">
+        <v>44158</v>
+      </c>
       <c r="F20" s="34"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
lesson #17 video records uploaded on youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -150,6 +150,10 @@
   </si>
   <si>
     <t xml:space="preserve">OOP #4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part #1: https://youtu.be/DeTDHgl6Y-Q
+Part #2: https://youtu.be/TeLokMw1VyQ</t>
   </si>
 </sst>
 </file>
@@ -542,7 +546,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -889,7 +893,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="28.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="34"/>
       <c r="B20" s="35" t="n">
         <v>17</v>
@@ -903,7 +907,9 @@
       <c r="E20" s="15" t="n">
         <v>44158</v>
       </c>
-      <c r="F20" s="34"/>
+      <c r="F20" s="36" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="35" t="n">

</xml_diff>

<commit_message>
lesson #18 lesson code attached
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -546,7 +546,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -893,7 +893,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="28.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="34"/>
       <c r="B20" s="35" t="n">
         <v>17</v>
@@ -916,6 +916,9 @@
         <v>18</v>
       </c>
       <c r="C21" s="36"/>
+      <c r="E21" s="15" t="n">
+        <v>44163</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="35" t="n">

</xml_diff>

<commit_message>
lesson #20 lesson video record uploaded into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://youtu.be/WZK0AT6SJfk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OOP #7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/XBw5dgHg3dE</t>
   </si>
 </sst>
 </file>
@@ -259,7 +265,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -270,6 +276,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -324,7 +336,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -357,19 +369,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -377,54 +389,74 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -465,20 +497,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -489,8 +513,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -573,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -608,7 +632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
@@ -628,7 +652,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12"/>
       <c r="B3" s="8" t="n">
         <f aca="false">B2+1</f>
@@ -647,7 +671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12"/>
       <c r="B4" s="8" t="n">
         <f aca="false">B3+1</f>
@@ -666,7 +690,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="25.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12"/>
       <c r="B5" s="8" t="n">
         <f aca="false">B4+1</f>
@@ -685,7 +709,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="25.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12"/>
       <c r="B6" s="8" t="n">
         <f aca="false">B5+1</f>
@@ -704,7 +728,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12"/>
       <c r="B7" s="8" t="n">
         <f aca="false">B6+1</f>
@@ -723,7 +747,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18"/>
       <c r="B8" s="19" t="n">
         <v>7</v>
@@ -741,7 +765,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" s="24" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="25" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="21"/>
       <c r="B9" s="22" t="n">
         <v>8</v>
@@ -749,7 +773,7 @@
       <c r="C9" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="22" t="n">
+      <c r="D9" s="24" t="n">
         <v>2</v>
       </c>
       <c r="E9" s="15" t="n">
@@ -761,267 +785,285 @@
     </row>
     <row r="10" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="18"/>
-      <c r="B10" s="19" t="n">
+      <c r="B10" s="26" t="n">
         <v>9</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="19" t="n">
-        <v>2</v>
-      </c>
-      <c r="E10" s="15" t="n">
+      <c r="D10" s="26" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" s="28" t="n">
         <v>44128</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="27" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="18"/>
-      <c r="B11" s="19" t="n">
+      <c r="B11" s="26" t="n">
         <v>10</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="19" t="n">
-        <v>2</v>
-      </c>
-      <c r="E11" s="15" t="n">
+      <c r="D11" s="26" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" s="28" t="n">
         <v>44132</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="30" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="18"/>
-      <c r="B12" s="19" t="n">
+      <c r="B12" s="26" t="n">
         <v>11</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="19" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" s="15" t="n">
+      <c r="D12" s="26" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" s="28" t="n">
         <v>44135</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" s="29" customFormat="true" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="26"/>
-      <c r="B13" s="19" t="n">
+    <row r="13" s="34" customFormat="true" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="31"/>
+      <c r="B13" s="26" t="n">
         <v>12</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="19" t="n">
-        <v>2</v>
-      </c>
-      <c r="E13" s="15" t="n">
+      <c r="D13" s="26" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" s="28" t="n">
         <v>44503</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="33" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="18"/>
-      <c r="B14" s="30" t="n">
+      <c r="B14" s="35" t="n">
         <v>13</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="30" t="n">
-        <v>2</v>
-      </c>
-      <c r="E14" s="32" t="n">
+      <c r="D14" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" s="37" t="n">
         <v>44142</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="30" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="18"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="33"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="38"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="34"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="34"/>
-    </row>
-    <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="34" t="s">
+      <c r="A16" s="39"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="39"/>
+    </row>
+    <row r="17" s="25" customFormat="true" ht="41.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="35" t="n">
+      <c r="B17" s="24" t="n">
         <v>14</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="35" t="n">
-        <v>2</v>
-      </c>
-      <c r="E17" s="38" t="n">
+      <c r="D17" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" s="15" t="n">
         <v>44144</v>
       </c>
-      <c r="F17" s="39" t="s">
+      <c r="F17" s="42" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="34"/>
-      <c r="B18" s="35" t="n">
+    <row r="18" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="39"/>
+      <c r="B18" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="35" t="n">
-        <v>2</v>
-      </c>
-      <c r="E18" s="38" t="n">
+      <c r="D18" s="19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" s="15" t="n">
         <v>44151</v>
       </c>
-      <c r="F18" s="36" t="s">
+      <c r="F18" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="34"/>
-      <c r="B19" s="35" t="n">
+    <row r="19" s="25" customFormat="true" ht="54.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="41"/>
+      <c r="B19" s="22" t="n">
         <v>16</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="C19" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="35" t="n">
-        <v>2</v>
-      </c>
-      <c r="E19" s="38" t="n">
+      <c r="D19" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" s="15" t="n">
         <v>44156</v>
       </c>
-      <c r="F19" s="36" t="s">
+      <c r="F19" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="34"/>
-      <c r="B20" s="35" t="n">
+      <c r="A20" s="39"/>
+      <c r="B20" s="19" t="n">
         <v>17</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="35" t="n">
-        <v>2</v>
-      </c>
-      <c r="E20" s="38" t="n">
+      <c r="D20" s="19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E20" s="15" t="n">
         <v>44158</v>
       </c>
-      <c r="F20" s="36" t="s">
+      <c r="F20" s="20" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="34"/>
-      <c r="B21" s="35" t="n">
+      <c r="A21" s="39"/>
+      <c r="B21" s="19" t="n">
         <v>18</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="35" t="n">
-        <v>2</v>
-      </c>
-      <c r="E21" s="38" t="n">
+      <c r="D21" s="19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E21" s="15" t="n">
         <v>44163</v>
       </c>
-      <c r="F21" s="34" t="s">
+      <c r="F21" s="39" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="34"/>
-      <c r="B22" s="35" t="n">
+      <c r="A22" s="39"/>
+      <c r="B22" s="19" t="n">
         <v>19</v>
       </c>
-      <c r="C22" s="36" t="s">
+      <c r="C22" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="35" t="n">
-        <v>3</v>
-      </c>
-      <c r="E22" s="38" t="n">
+      <c r="D22" s="19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E22" s="15" t="n">
         <v>44166</v>
       </c>
-      <c r="F22" s="40" t="s">
+      <c r="F22" s="43" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="34"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="34"/>
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="39"/>
+      <c r="B23" s="19" t="n">
+        <v>20</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E23" s="15" t="n">
+        <v>44170</v>
+      </c>
+      <c r="F23" s="39" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="34"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="34"/>
+      <c r="A24" s="39"/>
+      <c r="B24" s="19" t="n">
+        <v>21</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="39"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="34"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="34"/>
+      <c r="A25" s="39"/>
+      <c r="B25" s="19" t="n">
+        <v>22</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="39"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="34"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="34"/>
+      <c r="A26" s="39"/>
+      <c r="B26" s="19" t="n">
+        <v>23</v>
+      </c>
+      <c r="C26" s="20"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="39"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="34"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="34"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="44" t="n">
+        <v>24</v>
+      </c>
+      <c r="C27" s="20"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="39"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="34"/>
-      <c r="B28" s="35"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="34"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="39"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
lesson 21 video record uploaded into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -172,6 +172,15 @@
   </si>
   <si>
     <t xml:space="preserve">https://youtu.be/XBw5dgHg3dE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exceptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/fVmROnih-Io</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File I/O &amp; Date-Time API</t>
   </si>
 </sst>
 </file>
@@ -597,8 +606,8 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -608,7 +617,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="35.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="9.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="60.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="52.42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="9.14"/>
   </cols>
   <sheetData>
@@ -963,7 +972,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="39"/>
       <c r="B21" s="19" t="n">
         <v>18</v>
@@ -999,7 +1008,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="39"/>
       <c r="B23" s="19" t="n">
         <v>20</v>
@@ -1017,34 +1026,54 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="39"/>
       <c r="B24" s="19" t="n">
         <v>21</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="39"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E24" s="15" t="n">
+        <v>44173</v>
+      </c>
+      <c r="F24" s="39" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="39"/>
       <c r="B25" s="19" t="n">
         <v>22</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="24"/>
+      <c r="C25" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E25" s="15" t="n">
+        <v>44177</v>
+      </c>
       <c r="F25" s="39"/>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="39"/>
       <c r="B26" s="19" t="n">
         <v>23</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="24"/>
+      <c r="C26" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E26" s="15" t="n">
+        <v>44179</v>
+      </c>
       <c r="F26" s="39"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,7 +1105,10 @@
     <hyperlink ref="F8" r:id="rId7" display="https://youtu.be/GAIGLm6nZVI"/>
     <hyperlink ref="F11" r:id="rId8" location="5W1WODw_dXbtaLwv7hdQSQ" display="https://mega.nz/folder/99JXxCJB#5W1WODw_dXbtaLwv7hdQSQ"/>
     <hyperlink ref="F12" r:id="rId9" location="5W1WODw_dXbtaLwv7hdQSQ" display="https://mega.nz/folder/99JXxCJB#5W1WODw_dXbtaLwv7hdQSQ"/>
-    <hyperlink ref="F22" r:id="rId10" display="https://youtu.be/WZK0AT6SJfk"/>
+    <hyperlink ref="F21" r:id="rId10" display="https://youtu.be/1XCeWEAcA4I"/>
+    <hyperlink ref="F22" r:id="rId11" display="https://youtu.be/WZK0AT6SJfk"/>
+    <hyperlink ref="F23" r:id="rId12" display="https://youtu.be/XBw5dgHg3dE"/>
+    <hyperlink ref="F24" r:id="rId13" display="https://youtu.be/fVmROnih-Io"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson 22 lesson code, slide, output data attached!
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -181,6 +181,12 @@
   </si>
   <si>
     <t xml:space="preserve">File I/O &amp; Date-Time API</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java 8 (Stream API,)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java 8 continued</t>
   </si>
 </sst>
 </file>
@@ -606,8 +612,8 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -617,7 +623,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="35.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="9.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="52.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="52.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="9.14"/>
   </cols>
   <sheetData>
@@ -1066,7 +1072,7 @@
         <v>23</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="D26" s="19" t="n">
         <v>2</v>
@@ -1076,14 +1082,20 @@
       </c>
       <c r="F26" s="39"/>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="39"/>
       <c r="B27" s="44" t="n">
         <v>24</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="24"/>
+      <c r="C27" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" s="15" t="n">
+        <v>44184</v>
+      </c>
       <c r="F27" s="39"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
lesson 22 video record uploaded into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t xml:space="preserve">File I/O &amp; Date-Time API</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://join.skype.com/bNBYbKwuMugv</t>
   </si>
   <si>
     <t xml:space="preserve">Java 8 (Stream API,)</t>
@@ -613,7 +616,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1064,7 +1067,9 @@
       <c r="E25" s="15" t="n">
         <v>44177</v>
       </c>
-      <c r="F25" s="39"/>
+      <c r="F25" s="39" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="39"/>
@@ -1072,7 +1077,7 @@
         <v>23</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D26" s="19" t="n">
         <v>2</v>
@@ -1088,7 +1093,7 @@
         <v>24</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D27" s="19" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
lesson 23 video recording uploaded into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t xml:space="preserve">Java 8 (Stream API)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/T2PvF31diZY</t>
   </si>
   <si>
     <t xml:space="preserve">Java 8 continued, Section Project #1</t>
@@ -609,14 +612,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1071,7 +1074,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="39"/>
       <c r="B26" s="19" t="n">
         <v>23</v>
@@ -1085,7 +1088,9 @@
       <c r="E26" s="15" t="n">
         <v>44179</v>
       </c>
-      <c r="F26" s="39"/>
+      <c r="F26" s="39" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="39"/>
@@ -1093,7 +1098,7 @@
         <v>24</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D27" s="19" t="n">
         <v>2</v>
@@ -1127,6 +1132,7 @@
     <hyperlink ref="F23" r:id="rId12" display="https://youtu.be/XBw5dgHg3dE"/>
     <hyperlink ref="F24" r:id="rId13" display="https://youtu.be/fVmROnih-Io"/>
     <hyperlink ref="F25" r:id="rId14" display="https://youtu.be/CPQoVMBvaPo"/>
+    <hyperlink ref="F26" r:id="rId15" display="https://youtu.be/T2PvF31diZY"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson 24 video record on youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -192,7 +192,12 @@
     <t xml:space="preserve">https://youtu.be/T2PvF31diZY</t>
   </si>
   <si>
-    <t xml:space="preserve">Java 8 continued, Section Project #1</t>
+    <t xml:space="preserve">Java 8 continued, Step Project #1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part #1: https://youtu.be/seCQZfHx_bE
+Part #2: https://youtu.be/rT3auL6oukk
+Part #3: https://youtu.be/CPdlyJpnOCo</t>
   </si>
 </sst>
 </file>
@@ -357,7 +362,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -532,10 +537,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -618,8 +619,8 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1092,21 +1093,23 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="39"/>
-      <c r="B27" s="44" t="n">
+    <row r="27" s="25" customFormat="true" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="41"/>
+      <c r="B27" s="22" t="n">
         <v>24</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="19" t="n">
+      <c r="D27" s="24" t="n">
         <v>2</v>
       </c>
       <c r="E27" s="15" t="n">
         <v>44184</v>
       </c>
-      <c r="F27" s="39"/>
+      <c r="F27" s="23" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="39"/>

</xml_diff>

<commit_message>
lesson #25 class code attached
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -619,8 +619,8 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
lesson #25 class code and slide attached
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -192,12 +192,15 @@
     <t xml:space="preserve">https://youtu.be/T2PvF31diZY</t>
   </si>
   <si>
-    <t xml:space="preserve">Java 8 continued, Step Project #1</t>
+    <t xml:space="preserve">Java 8 continued</t>
   </si>
   <si>
     <t xml:space="preserve">Part #1: https://youtu.be/seCQZfHx_bE
 Part #2: https://youtu.be/rT3auL6oukk
 Part #3: https://youtu.be/CPdlyJpnOCo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step Project #1 explanation, Algorithms intro</t>
   </si>
 </sst>
 </file>
@@ -208,7 +211,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -289,6 +292,12 @@
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -362,7 +371,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -537,6 +546,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -619,8 +632,8 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B21" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1111,13 +1124,21 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="39"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="39"/>
+    <row r="28" s="25" customFormat="true" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="41"/>
+      <c r="B28" s="24" t="n">
+        <v>25</v>
+      </c>
+      <c r="C28" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E28" s="15" t="n">
+        <v>44191</v>
+      </c>
+      <c r="F28" s="41"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
lesson #25 video record uploaded into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t xml:space="preserve">Step Project #1 explanation, Algorithms intro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/SPljuXKqz_g</t>
   </si>
 </sst>
 </file>
@@ -211,7 +214,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -293,12 +296,6 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -371,7 +368,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -546,10 +543,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -633,7 +626,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B21" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
+      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1124,12 +1117,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" s="25" customFormat="true" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" s="25" customFormat="true" ht="27.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="41"/>
       <c r="B28" s="24" t="n">
         <v>25</v>
       </c>
-      <c r="C28" s="44" t="s">
+      <c r="C28" s="42" t="s">
         <v>55</v>
       </c>
       <c r="D28" s="24" t="n">
@@ -1138,7 +1131,9 @@
       <c r="E28" s="15" t="n">
         <v>44191</v>
       </c>
-      <c r="F28" s="41"/>
+      <c r="F28" s="41" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1157,6 +1152,7 @@
     <hyperlink ref="F24" r:id="rId13" display="https://youtu.be/fVmROnih-Io"/>
     <hyperlink ref="F25" r:id="rId14" display="https://youtu.be/CPQoVMBvaPo"/>
     <hyperlink ref="F26" r:id="rId15" display="https://youtu.be/T2PvF31diZY"/>
+    <hyperlink ref="F28" r:id="rId16" display="https://youtu.be/SPljuXKqz_g"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #26 lesson code attached and video record uploaded into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -200,10 +200,16 @@
 Part #3: https://youtu.be/CPdlyJpnOCo</t>
   </si>
   <si>
-    <t xml:space="preserve">Step Project #1 explanation, Algorithms intro</t>
+    <t xml:space="preserve">Step Project #1 explanation, Algorithms intro #1</t>
   </si>
   <si>
     <t xml:space="preserve">https://youtu.be/SPljuXKqz_g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step Project #1, Algorithms #2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/FDDtGyTHneA</t>
   </si>
 </sst>
 </file>
@@ -623,10 +629,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B21" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1117,9 +1123,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" s="25" customFormat="true" ht="27.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" s="25" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="41"/>
-      <c r="B28" s="24" t="n">
+      <c r="B28" s="22" t="n">
         <v>25</v>
       </c>
       <c r="C28" s="42" t="s">
@@ -1135,6 +1141,59 @@
         <v>56</v>
       </c>
     </row>
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="41"/>
+      <c r="B29" s="24" t="n">
+        <v>26</v>
+      </c>
+      <c r="C29" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" s="15" t="n">
+        <v>44200</v>
+      </c>
+      <c r="F29" s="41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="24" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="24" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="24" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="24" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="24" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="22" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="24"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="https://youtu.be/3Q7s1cpByuk"/>
@@ -1153,6 +1212,7 @@
     <hyperlink ref="F25" r:id="rId14" display="https://youtu.be/CPQoVMBvaPo"/>
     <hyperlink ref="F26" r:id="rId15" display="https://youtu.be/T2PvF31diZY"/>
     <hyperlink ref="F28" r:id="rId16" display="https://youtu.be/SPljuXKqz_g"/>
+    <hyperlink ref="F29" r:id="rId17" display="https://youtu.be/FDDtGyTHneA"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #27 video record uploaded into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -210,6 +210,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://youtu.be/FDDtGyTHneA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step Project #1, Algorithms #3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/uJR7GhziAKs </t>
   </si>
 </sst>
 </file>
@@ -632,7 +638,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1159,9 +1165,21 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="24" t="n">
         <v>27</v>
+      </c>
+      <c r="C30" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E30" s="15" t="n">
+        <v>44202</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
lesson #28 class code and slide attached
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -212,10 +212,13 @@
     <t xml:space="preserve">https://youtu.be/FDDtGyTHneA</t>
   </si>
   <si>
-    <t xml:space="preserve">Step Project #1, Algorithms #3</t>
+    <t xml:space="preserve">Algorithms #3</t>
   </si>
   <si>
     <t xml:space="preserve">https://youtu.be/uJR7GhziAKs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Structures #1</t>
   </si>
 </sst>
 </file>
@@ -638,7 +641,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
+      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1172,7 +1175,7 @@
       <c r="C30" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="D30" s="2" t="n">
+      <c r="D30" s="24" t="n">
         <v>2</v>
       </c>
       <c r="E30" s="15" t="n">
@@ -1182,9 +1185,18 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="24" t="n">
         <v>28</v>
+      </c>
+      <c r="C31" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E31" s="15" t="n">
+        <v>44205</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
lesson #28 video record uploaded into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -218,7 +218,22 @@
     <t xml:space="preserve">https://youtu.be/uJR7GhziAKs </t>
   </si>
   <si>
-    <t xml:space="preserve">Data Structures #1</t>
+    <t xml:space="preserve">Data Structures, Collection API</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/NyXBevtFNSc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database intro #1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database #2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database #3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recap + part #1 final exam</t>
   </si>
 </sst>
 </file>
@@ -332,7 +347,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -354,6 +369,13 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -383,7 +405,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -558,6 +580,22 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -640,8 +678,8 @@
   </sheetPr>
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1181,11 +1219,11 @@
       <c r="E30" s="15" t="n">
         <v>44202</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="39" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="24" t="n">
         <v>28</v>
       </c>
@@ -1198,29 +1236,76 @@
       <c r="E31" s="15" t="n">
         <v>44205</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F31" s="39" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="24" t="n">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E32" s="15" t="n">
+        <v>44208</v>
+      </c>
+      <c r="F32" s="39"/>
+    </row>
+    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="24" t="n">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E33" s="15" t="n">
+        <v>44212</v>
+      </c>
+      <c r="F33" s="39"/>
+    </row>
+    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="24" t="n">
         <v>31</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E34" s="15" t="n">
+        <v>44215</v>
+      </c>
+      <c r="F34" s="39"/>
+    </row>
+    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="22" t="n">
         <v>32</v>
       </c>
+      <c r="C35" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E35" s="15" t="n">
+        <v>44219</v>
+      </c>
+      <c r="F35" s="39"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="24"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="47"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1243,6 +1328,7 @@
     <hyperlink ref="F26" r:id="rId15" display="https://youtu.be/T2PvF31diZY"/>
     <hyperlink ref="F28" r:id="rId16" display="https://youtu.be/SPljuXKqz_g"/>
     <hyperlink ref="F29" r:id="rId17" display="https://youtu.be/FDDtGyTHneA"/>
+    <hyperlink ref="F31" r:id="rId18" display="https://youtu.be/NyXBevtFNSc"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #29 video record uploaded into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -215,7 +215,7 @@
     <t xml:space="preserve">Algorithms #3</t>
   </si>
   <si>
-    <t xml:space="preserve">https://youtu.be/uJR7GhziAKs </t>
+    <t xml:space="preserve">https://youtu.be/uJR7GhziAKs</t>
   </si>
   <si>
     <t xml:space="preserve">Data Structures, Collection API</t>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t xml:space="preserve">Database intro #1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/lkg29JtG-r8 </t>
   </si>
   <si>
     <t xml:space="preserve">Database #2</t>
@@ -679,7 +682,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
+      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1253,14 +1256,16 @@
       <c r="E32" s="15" t="n">
         <v>44208</v>
       </c>
-      <c r="F32" s="39"/>
+      <c r="F32" s="39" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="24" t="n">
         <v>30</v>
       </c>
       <c r="C33" s="42" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D33" s="24" t="n">
         <v>2</v>
@@ -1275,7 +1280,7 @@
         <v>31</v>
       </c>
       <c r="C34" s="42" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D34" s="24" t="n">
         <v>2</v>
@@ -1290,7 +1295,7 @@
         <v>32</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D35" s="2" t="n">
         <v>2</v>
@@ -1328,7 +1333,9 @@
     <hyperlink ref="F26" r:id="rId15" display="https://youtu.be/T2PvF31diZY"/>
     <hyperlink ref="F28" r:id="rId16" display="https://youtu.be/SPljuXKqz_g"/>
     <hyperlink ref="F29" r:id="rId17" display="https://youtu.be/FDDtGyTHneA"/>
-    <hyperlink ref="F31" r:id="rId18" display="https://youtu.be/NyXBevtFNSc"/>
+    <hyperlink ref="F30" r:id="rId18" display="https://youtu.be/uJR7GhziAKs"/>
+    <hyperlink ref="F31" r:id="rId19" display="https://youtu.be/NyXBevtFNSc "/>
+    <hyperlink ref="F32" r:id="rId20" display="https://youtu.be/lkg29JtG-r8"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #30 video record uploaded into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -233,7 +233,10 @@
     <t xml:space="preserve">Database #2</t>
   </si>
   <si>
-    <t xml:space="preserve">Database #3</t>
+    <t xml:space="preserve">https://youtu.be/XLAimCkUnx8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database #3 – JDBC</t>
   </si>
   <si>
     <t xml:space="preserve">Recap + part #1 final exam</t>
@@ -681,8 +684,8 @@
   </sheetPr>
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1260,7 +1263,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="24" t="n">
         <v>30</v>
       </c>
@@ -1271,16 +1274,18 @@
         <v>2</v>
       </c>
       <c r="E33" s="15" t="n">
-        <v>44212</v>
-      </c>
-      <c r="F33" s="39"/>
+        <v>44211</v>
+      </c>
+      <c r="F33" s="39" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="24" t="n">
         <v>31</v>
       </c>
       <c r="C34" s="42" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D34" s="24" t="n">
         <v>2</v>
@@ -1295,7 +1300,7 @@
         <v>32</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D35" s="2" t="n">
         <v>2</v>
@@ -1335,7 +1340,8 @@
     <hyperlink ref="F29" r:id="rId17" display="https://youtu.be/FDDtGyTHneA"/>
     <hyperlink ref="F30" r:id="rId18" display="https://youtu.be/uJR7GhziAKs"/>
     <hyperlink ref="F31" r:id="rId19" display="https://youtu.be/NyXBevtFNSc "/>
-    <hyperlink ref="F32" r:id="rId20" display="https://youtu.be/lkg29JtG-r8"/>
+    <hyperlink ref="F32" r:id="rId20" display="https://youtu.be/lkg29JtG-r8 "/>
+    <hyperlink ref="F33" r:id="rId21" display="https://youtu.be/XLAimCkUnx8"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #31 video record uploaded into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t xml:space="preserve">Database #3 – JDBC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/utmdGTOnRm8 </t>
   </si>
   <si>
     <t xml:space="preserve">Recap + part #1 final exam</t>
@@ -685,7 +688,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1280,7 +1283,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="24" t="n">
         <v>31</v>
       </c>
@@ -1293,14 +1296,16 @@
       <c r="E34" s="15" t="n">
         <v>44215</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="39" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="22" t="n">
         <v>32</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D35" s="2" t="n">
         <v>2</v>
@@ -1341,7 +1346,8 @@
     <hyperlink ref="F30" r:id="rId18" display="https://youtu.be/uJR7GhziAKs"/>
     <hyperlink ref="F31" r:id="rId19" display="https://youtu.be/NyXBevtFNSc "/>
     <hyperlink ref="F32" r:id="rId20" display="https://youtu.be/lkg29JtG-r8 "/>
-    <hyperlink ref="F33" r:id="rId21" display="https://youtu.be/XLAimCkUnx8"/>
+    <hyperlink ref="F33" r:id="rId21" display="https://youtu.be/XLAimCkUnx8 "/>
+    <hyperlink ref="F34" r:id="rId22" display="https://youtu.be/utmdGTOnRm8"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #32 syllabus polished a bit
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -236,31 +236,16 @@
     <t xml:space="preserve">https://youtu.be/XLAimCkUnx8 </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Database #3 – JDBC, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Recap</t>
-    </r>
+    <t xml:space="preserve">Database #3 – JDBC, Recap</t>
   </si>
   <si>
     <t xml:space="preserve">https://youtu.be/utmdGTOnRm8 </t>
   </si>
   <si>
     <t xml:space="preserve">Recap + web intro (java EE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/Pl6MA-l9c_8 </t>
   </si>
 </sst>
 </file>
@@ -271,7 +256,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -353,12 +338,6 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -712,7 +691,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
+      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1324,7 +1303,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="22" t="n">
         <v>32</v>
       </c>
@@ -1337,7 +1316,9 @@
       <c r="E35" s="15" t="n">
         <v>44219</v>
       </c>
-      <c r="F35" s="39"/>
+      <c r="F35" s="39" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="24"/>
@@ -1372,6 +1353,7 @@
     <hyperlink ref="F32" r:id="rId20" display="https://youtu.be/lkg29JtG-r8 "/>
     <hyperlink ref="F33" r:id="rId21" display="https://youtu.be/XLAimCkUnx8 "/>
     <hyperlink ref="F34" r:id="rId22" display="https://youtu.be/utmdGTOnRm8 "/>
+    <hyperlink ref="F35" r:id="rId23" display="https://youtu.be/Pl6MA-l9c_8"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #34 lesson code attached
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -246,6 +246,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://youtu.be/Pl6MA-l9c_8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java EE – Servlet handler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freemarker</t>
   </si>
 </sst>
 </file>
@@ -688,10 +694,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1327,8 +1333,100 @@
       <c r="E36" s="46"/>
       <c r="F36" s="47"/>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="22" t="n">
+        <v>33</v>
+      </c>
+      <c r="C37" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E37" s="15" t="n">
+        <v>44225</v>
+      </c>
+      <c r="F37" s="41"/>
+    </row>
+    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="24" t="n">
+        <v>34</v>
+      </c>
+      <c r="C38" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E38" s="15" t="n">
+        <v>44226</v>
+      </c>
+      <c r="F38" s="41"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="24" t="n">
+        <v>35</v>
+      </c>
+      <c r="C39" s="42"/>
+      <c r="D39" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E39" s="15"/>
+      <c r="F39" s="39"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="24" t="n">
+        <v>36</v>
+      </c>
+      <c r="C40" s="42"/>
+      <c r="D40" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E40" s="15"/>
+      <c r="F40" s="39"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="24" t="n">
+        <v>37</v>
+      </c>
+      <c r="D41" s="19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E41" s="15"/>
+      <c r="F41" s="39"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="24" t="n">
+        <v>38</v>
+      </c>
+      <c r="C42" s="42"/>
+      <c r="D42" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E42" s="15"/>
+      <c r="F42" s="39"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="24" t="n">
+        <v>39</v>
+      </c>
+      <c r="C43" s="42"/>
+      <c r="D43" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E43" s="15"/>
+      <c r="F43" s="39"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="22" t="n">
+        <v>40</v>
+      </c>
+      <c r="D44" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E44" s="15"/>
+      <c r="F44" s="39"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="https://youtu.be/3Q7s1cpByuk"/>
@@ -1353,7 +1451,7 @@
     <hyperlink ref="F32" r:id="rId20" display="https://youtu.be/lkg29JtG-r8 "/>
     <hyperlink ref="F33" r:id="rId21" display="https://youtu.be/XLAimCkUnx8 "/>
     <hyperlink ref="F34" r:id="rId22" display="https://youtu.be/utmdGTOnRm8 "/>
-    <hyperlink ref="F35" r:id="rId23" display="https://youtu.be/Pl6MA-l9c_8"/>
+    <hyperlink ref="F35" r:id="rId23" display="https://youtu.be/Pl6MA-l9c_8 "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #34 video record uploaded into youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -251,7 +251,13 @@
     <t xml:space="preserve">Java EE – Servlet handler</t>
   </si>
   <si>
+    <t xml:space="preserve">https://youtu.be/dbPUQE2NsLo </t>
+  </si>
+  <si>
     <t xml:space="preserve">Freemarker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/IAOZ1-2VPuQ </t>
   </si>
 </sst>
 </file>
@@ -697,7 +703,7 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
+      <selection pane="topLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1333,7 +1339,7 @@
       <c r="E36" s="46"/>
       <c r="F36" s="47"/>
     </row>
-    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="22" t="n">
         <v>33</v>
       </c>
@@ -1346,14 +1352,16 @@
       <c r="E37" s="15" t="n">
         <v>44225</v>
       </c>
-      <c r="F37" s="41"/>
-    </row>
-    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F37" s="41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="24" t="n">
         <v>34</v>
       </c>
       <c r="C38" s="42" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D38" s="24" t="n">
         <v>2</v>
@@ -1361,16 +1369,16 @@
       <c r="E38" s="15" t="n">
         <v>44226</v>
       </c>
-      <c r="F38" s="41"/>
+      <c r="F38" s="41" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="24" t="n">
         <v>35</v>
       </c>
       <c r="C39" s="42"/>
-      <c r="D39" s="24" t="n">
-        <v>2</v>
-      </c>
+      <c r="D39" s="24"/>
       <c r="E39" s="15"/>
       <c r="F39" s="39"/>
     </row>
@@ -1379,9 +1387,7 @@
         <v>36</v>
       </c>
       <c r="C40" s="42"/>
-      <c r="D40" s="24" t="n">
-        <v>2</v>
-      </c>
+      <c r="D40" s="24"/>
       <c r="E40" s="15"/>
       <c r="F40" s="39"/>
     </row>
@@ -1389,9 +1395,7 @@
       <c r="B41" s="24" t="n">
         <v>37</v>
       </c>
-      <c r="D41" s="19" t="n">
-        <v>2</v>
-      </c>
+      <c r="D41" s="19"/>
       <c r="E41" s="15"/>
       <c r="F41" s="39"/>
     </row>
@@ -1400,9 +1404,7 @@
         <v>38</v>
       </c>
       <c r="C42" s="42"/>
-      <c r="D42" s="24" t="n">
-        <v>2</v>
-      </c>
+      <c r="D42" s="24"/>
       <c r="E42" s="15"/>
       <c r="F42" s="39"/>
     </row>
@@ -1411,9 +1413,7 @@
         <v>39</v>
       </c>
       <c r="C43" s="42"/>
-      <c r="D43" s="24" t="n">
-        <v>2</v>
-      </c>
+      <c r="D43" s="24"/>
       <c r="E43" s="15"/>
       <c r="F43" s="39"/>
     </row>
@@ -1421,9 +1421,8 @@
       <c r="B44" s="22" t="n">
         <v>40</v>
       </c>
-      <c r="D44" s="2" t="n">
-        <v>2</v>
-      </c>
+      <c r="C44" s="42"/>
+      <c r="D44" s="24"/>
       <c r="E44" s="15"/>
       <c r="F44" s="39"/>
     </row>
@@ -1452,6 +1451,8 @@
     <hyperlink ref="F33" r:id="rId21" display="https://youtu.be/XLAimCkUnx8 "/>
     <hyperlink ref="F34" r:id="rId22" display="https://youtu.be/utmdGTOnRm8 "/>
     <hyperlink ref="F35" r:id="rId23" display="https://youtu.be/Pl6MA-l9c_8 "/>
+    <hyperlink ref="F37" r:id="rId24" display="https://youtu.be/dbPUQE2NsLo"/>
+    <hyperlink ref="F38" r:id="rId25" display="https://youtu.be/IAOZ1-2VPuQ"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #35 video record on youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -258,6 +258,15 @@
   </si>
   <si>
     <t xml:space="preserve">https://youtu.be/IAOZ1-2VPuQ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transactions, Cookies, Filters,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/bNLYRnJj6R0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serialization, JSON, XML</t>
   </si>
 </sst>
 </file>
@@ -702,8 +711,8 @@
   </sheetPr>
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1356,7 +1365,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="24" t="n">
         <v>34</v>
       </c>
@@ -1373,21 +1382,33 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="24" t="n">
         <v>35</v>
       </c>
-      <c r="C39" s="42"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="39"/>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E39" s="15" t="n">
+        <v>44229</v>
+      </c>
+      <c r="F39" s="39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="24" t="n">
         <v>36</v>
       </c>
-      <c r="C40" s="42"/>
-      <c r="D40" s="24"/>
+      <c r="C40" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" s="24" t="n">
+        <v>2</v>
+      </c>
       <c r="E40" s="15"/>
       <c r="F40" s="39"/>
     </row>
@@ -1451,8 +1472,9 @@
     <hyperlink ref="F33" r:id="rId21" display="https://youtu.be/XLAimCkUnx8 "/>
     <hyperlink ref="F34" r:id="rId22" display="https://youtu.be/utmdGTOnRm8 "/>
     <hyperlink ref="F35" r:id="rId23" display="https://youtu.be/Pl6MA-l9c_8 "/>
-    <hyperlink ref="F37" r:id="rId24" display="https://youtu.be/dbPUQE2NsLo"/>
-    <hyperlink ref="F38" r:id="rId25" display="https://youtu.be/IAOZ1-2VPuQ"/>
+    <hyperlink ref="F37" r:id="rId24" display="https://youtu.be/dbPUQE2NsLo "/>
+    <hyperlink ref="F38" r:id="rId25" display="https://youtu.be/IAOZ1-2VPuQ "/>
+    <hyperlink ref="F39" r:id="rId26" display="https://youtu.be/bNLYRnJj6R0 "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #36 video record on youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t xml:space="preserve">Serialization, JSON, XML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/RGowh6wcrFo </t>
   </si>
 </sst>
 </file>
@@ -711,8 +714,8 @@
   </sheetPr>
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B22" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1409,8 +1412,12 @@
       <c r="D40" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="E40" s="15"/>
-      <c r="F40" s="39"/>
+      <c r="E40" s="15" t="n">
+        <v>44232</v>
+      </c>
+      <c r="F40" s="39" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="24" t="n">
@@ -1475,6 +1482,7 @@
     <hyperlink ref="F37" r:id="rId24" display="https://youtu.be/dbPUQE2NsLo "/>
     <hyperlink ref="F38" r:id="rId25" display="https://youtu.be/IAOZ1-2VPuQ "/>
     <hyperlink ref="F39" r:id="rId26" display="https://youtu.be/bNLYRnJj6R0 "/>
+    <hyperlink ref="F40" r:id="rId27" display="https://youtu.be/RGowh6wcrFo"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #37 lesson code in youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -715,7 +715,7 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B22" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
+      <selection pane="topLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1423,7 +1423,9 @@
       <c r="B41" s="24" t="n">
         <v>37</v>
       </c>
-      <c r="D41" s="19"/>
+      <c r="D41" s="19" t="n">
+        <v>2</v>
+      </c>
       <c r="E41" s="15"/>
       <c r="F41" s="39"/>
     </row>
@@ -1482,7 +1484,7 @@
     <hyperlink ref="F37" r:id="rId24" display="https://youtu.be/dbPUQE2NsLo "/>
     <hyperlink ref="F38" r:id="rId25" display="https://youtu.be/IAOZ1-2VPuQ "/>
     <hyperlink ref="F39" r:id="rId26" display="https://youtu.be/bNLYRnJj6R0 "/>
-    <hyperlink ref="F40" r:id="rId27" display="https://youtu.be/RGowh6wcrFo"/>
+    <hyperlink ref="F40" r:id="rId27" display="https://youtu.be/RGowh6wcrFo "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson #40 lesson video record on youtube
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="91">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -297,6 +297,15 @@
   </si>
   <si>
     <t xml:space="preserve">Spring intro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/E3LZMBqVjQQ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spring MVC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/AJnCbBv3o3o </t>
   </si>
 </sst>
 </file>
@@ -746,7 +755,7 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
+      <selection pane="topLeft" activeCell="F47" activeCellId="0" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1492,7 +1501,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>86</v>
       </c>
@@ -1506,16 +1515,18 @@
         <v>2</v>
       </c>
       <c r="E43" s="15" t="n">
-        <v>44243</v>
-      </c>
-      <c r="F43" s="39"/>
+        <v>44245</v>
+      </c>
+      <c r="F43" s="39" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="22" t="n">
         <v>40</v>
       </c>
       <c r="C44" s="42" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D44" s="24" t="n">
         <v>2</v>
@@ -1523,7 +1534,9 @@
       <c r="E44" s="15" t="n">
         <v>44246</v>
       </c>
-      <c r="F44" s="39"/>
+      <c r="F44" s="39" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1555,7 +1568,9 @@
     <hyperlink ref="F39" r:id="rId26" display="https://youtu.be/bNLYRnJj6R0 "/>
     <hyperlink ref="F40" r:id="rId27" display="https://youtu.be/RGowh6wcrFo "/>
     <hyperlink ref="F41" r:id="rId28" display="https://youtu.be/nJCTSjW0hQM "/>
-    <hyperlink ref="F42" r:id="rId29" display="https://youtu.be/tVDrwZ32lOk"/>
+    <hyperlink ref="F42" r:id="rId29" display="https://youtu.be/tVDrwZ32lOk "/>
+    <hyperlink ref="F43" r:id="rId30" display="https://youtu.be/E3LZMBqVjQQ"/>
+    <hyperlink ref="F44" r:id="rId31" display="https://youtu.be/AJnCbBv3o3o"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
lesson 40 topics attached
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -748,17 +748,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F47" activeCellId="0" sqref="F47"/>
+      <selection pane="topLeft" activeCell="B55" activeCellId="0" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="3.7"/>
@@ -1536,6 +1536,100 @@
       </c>
       <c r="F44" s="39" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="22" t="n">
+        <v>41</v>
+      </c>
+      <c r="C46" s="42"/>
+      <c r="D46" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E46" s="15"/>
+      <c r="F46" s="41"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="24" t="n">
+        <v>443</v>
+      </c>
+      <c r="C47" s="42"/>
+      <c r="D47" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E47" s="15"/>
+      <c r="F47" s="41"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="24" t="n">
+        <v>44</v>
+      </c>
+      <c r="C48" s="42"/>
+      <c r="D48" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E48" s="15"/>
+      <c r="F48" s="39"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="24" t="n">
+        <v>45</v>
+      </c>
+      <c r="C49" s="42"/>
+      <c r="D49" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E49" s="15"/>
+      <c r="F49" s="39"/>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="24" t="n">
+        <v>46</v>
+      </c>
+      <c r="C50" s="48"/>
+      <c r="D50" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E50" s="15"/>
+      <c r="F50" s="41"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="24" t="n">
+        <v>47</v>
+      </c>
+      <c r="C51" s="42"/>
+      <c r="D51" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E51" s="15"/>
+      <c r="F51" s="39"/>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="24" t="n">
+        <v>48</v>
+      </c>
+      <c r="C52" s="42"/>
+      <c r="D52" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E52" s="15"/>
+      <c r="F52" s="39"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="24" t="n">
+        <v>49</v>
+      </c>
+      <c r="C53" s="42"/>
+      <c r="D53" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E53" s="15"/>
+      <c r="F53" s="39"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="22" t="n">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1569,8 +1663,8 @@
     <hyperlink ref="F40" r:id="rId27" display="https://youtu.be/RGowh6wcrFo "/>
     <hyperlink ref="F41" r:id="rId28" display="https://youtu.be/nJCTSjW0hQM "/>
     <hyperlink ref="F42" r:id="rId29" display="https://youtu.be/tVDrwZ32lOk "/>
-    <hyperlink ref="F43" r:id="rId30" display="https://youtu.be/E3LZMBqVjQQ"/>
-    <hyperlink ref="F44" r:id="rId31" display="https://youtu.be/AJnCbBv3o3o"/>
+    <hyperlink ref="F43" r:id="rId30" display="https://youtu.be/E3LZMBqVjQQ "/>
+    <hyperlink ref="F44" r:id="rId31" display="https://youtu.be/AJnCbBv3o3o "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
course details updated and in the future will be closed for public, enough being social :)
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/course_details.xlsx
+++ b/src/main/java/org/eminera/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -318,9 +318,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://youtu.be/NSTbUammchE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spring data jpa, h2 database #2</t>
   </si>
 </sst>
 </file>
@@ -329,7 +326,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="d\-mmm\-yy"/>
+    <numFmt numFmtId="165" formatCode="D\-MMM\-YY"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -691,13 +688,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -767,13 +764,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C48" activeCellId="0" sqref="C48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E50" activeCellId="0" sqref="E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="3.7"/>
@@ -781,7 +778,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="9.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="15.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="52.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1587,77 +1584,6 @@
       <c r="F47" s="41" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="24" t="n">
-        <v>43</v>
-      </c>
-      <c r="C48" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="D48" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="E48" s="15"/>
-      <c r="F48" s="39"/>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="24" t="n">
-        <v>44</v>
-      </c>
-      <c r="C49" s="42"/>
-      <c r="D49" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="E49" s="15"/>
-      <c r="F49" s="39"/>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="24" t="n">
-        <v>45</v>
-      </c>
-      <c r="C50" s="48"/>
-      <c r="D50" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="E50" s="15"/>
-      <c r="F50" s="41"/>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="24" t="n">
-        <v>46</v>
-      </c>
-      <c r="C51" s="42"/>
-      <c r="D51" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="E51" s="15"/>
-      <c r="F51" s="39"/>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="24" t="n">
-        <v>47</v>
-      </c>
-      <c r="C52" s="42"/>
-      <c r="D52" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="E52" s="15"/>
-      <c r="F52" s="39"/>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="22" t="n">
-        <v>48</v>
-      </c>
-      <c r="C53" s="42"/>
-      <c r="D53" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="E53" s="15"/>
-      <c r="F53" s="39"/>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="0"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1692,8 +1618,8 @@
     <hyperlink ref="F42" r:id="rId29" display="https://youtu.be/tVDrwZ32lOk "/>
     <hyperlink ref="F43" r:id="rId30" display="https://youtu.be/E3LZMBqVjQQ "/>
     <hyperlink ref="F44" r:id="rId31" display="https://youtu.be/AJnCbBv3o3o "/>
-    <hyperlink ref="F46" r:id="rId32" display="https://youtu.be/W7j9-1PfVgg"/>
-    <hyperlink ref="F47" r:id="rId33" display="https://youtu.be/NSTbUammchE"/>
+    <hyperlink ref="F46" r:id="rId32" display="https://youtu.be/W7j9-1PfVgg "/>
+    <hyperlink ref="F47" r:id="rId33" display="https://youtu.be/NSTbUammchE "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>